<commit_message>
Final package 11 updates
</commit_message>
<xml_diff>
--- a/curation/BC_Package_R11_UR.xlsx
+++ b/curation/BC_Package_R11_UR.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\cdisc-org\COSMoS\curation\draft\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\cdisc-org\COSMoS\curation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{928C4527-F5E5-4362-A98A-0859BE5D3A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF728178-5C17-4559-88C7-1E5F3995E227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4155,9 +4155,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E7362A4-AAA0-4A03-8CD1-791B7A3B97E4}">
   <dimension ref="A1:AI95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T3" sqref="T3"/>
+      <selection pane="bottomLeft" activeCell="V60" sqref="V60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5665,7 +5665,7 @@
         <v>36</v>
       </c>
       <c r="S19" s="22" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="T19" s="22" t="s">
         <v>199</v>
@@ -5674,7 +5674,7 @@
         <v>200</v>
       </c>
       <c r="V19" s="22" t="s">
-        <v>99</v>
+        <v>226</v>
       </c>
       <c r="W19" s="22"/>
       <c r="X19" s="26" t="s">
@@ -7909,7 +7909,7 @@
         <v>36</v>
       </c>
       <c r="S48" s="22" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="T48" s="22" t="s">
         <v>199</v>
@@ -7918,7 +7918,7 @@
         <v>200</v>
       </c>
       <c r="V48" s="22" t="s">
-        <v>99</v>
+        <v>226</v>
       </c>
       <c r="W48" s="22"/>
       <c r="X48" s="26" t="s">
@@ -8848,7 +8848,7 @@
         <v>36</v>
       </c>
       <c r="S60" s="22" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="T60" s="22" t="s">
         <v>199</v>
@@ -8857,7 +8857,7 @@
         <v>200</v>
       </c>
       <c r="V60" s="22" t="s">
-        <v>99</v>
+        <v>226</v>
       </c>
       <c r="W60" s="22"/>
       <c r="X60" s="26" t="s">

</xml_diff>